<commit_message>
Refactor RAG pipeline to use token-based text splitter and enhance prompt testing; added debug prints for document retrieval need to fix truncation of API link
</commit_message>
<xml_diff>
--- a/app/isaac_resume_data.xlsx
+++ b/app/isaac_resume_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac.Tay\Code\Ask-Your-PDF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Izack Tay\Code\Ask-Your-PDF\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C9CB3D0-A5FC-4324-986B-728E62D3D422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92934553-71A5-45D1-8A2C-3B203ABD3D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65557E08-5C8B-4767-970E-1B56BB7B2868}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65557E08-5C8B-4767-970E-1B56BB7B2868}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,16 +448,16 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -465,7 +465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -473,7 +473,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>